<commit_message>
feat: firmware now is idempotent
</commit_message>
<xml_diff>
--- a/devices.xlsx
+++ b/devices.xlsx
@@ -1,29 +1,239 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soyel\OneDrive\Documents\Thermoguard\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A5EA42-EBE4-4274-9B65-30BF5814E548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="12048" yWindow="3072" windowWidth="9960" windowHeight="9972" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Devices" sheetId="1" r:id="rId1"/>
+    <sheet name="Clients" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="53">
+  <si>
+    <t>SERIAL_NUMBER</t>
+  </si>
+  <si>
+    <t>DEV_EUI</t>
+  </si>
+  <si>
+    <t>VOLTAGE_MEASURED</t>
+  </si>
+  <si>
+    <t>VOLTAGE_REPORTED</t>
+  </si>
+  <si>
+    <t>CLIENT</t>
+  </si>
+  <si>
+    <t>CLIENT_ID</t>
+  </si>
+  <si>
+    <t>70B3D57ED00728BF</t>
+  </si>
+  <si>
+    <t>70B3D57ED00728E3</t>
+  </si>
+  <si>
+    <t>70B3D57ED00728E4</t>
+  </si>
+  <si>
+    <t>70B3D57ED00728E5</t>
+  </si>
+  <si>
+    <t>70B3D57ED00728E6</t>
+  </si>
+  <si>
+    <t>70B3D57ED00728E7</t>
+  </si>
+  <si>
+    <t>70B3D57ED00728E8</t>
+  </si>
+  <si>
+    <t>70B3D57ED00728E9</t>
+  </si>
+  <si>
+    <t>70B3D57ED00728EA</t>
+  </si>
+  <si>
+    <t>70B3D57ED00728EB</t>
+  </si>
+  <si>
+    <t>70B3D57ED00728EC</t>
+  </si>
+  <si>
+    <t>70B3D57ED00728ED</t>
+  </si>
+  <si>
+    <t>70B3D57ED00728EE</t>
+  </si>
+  <si>
+    <t>70B3D57ED00728EF</t>
+  </si>
+  <si>
+    <t>70B3D57ED00728F0</t>
+  </si>
+  <si>
+    <t>APP_KEY</t>
+  </si>
+  <si>
+    <t>GR-0001</t>
+  </si>
+  <si>
+    <t>GR-0002</t>
+  </si>
+  <si>
+    <t>GR-0004</t>
+  </si>
+  <si>
+    <t>TEST-0001</t>
+  </si>
+  <si>
+    <t>TEST-0002</t>
+  </si>
+  <si>
+    <t>TEST-0003</t>
+  </si>
+  <si>
+    <t>TEST-0004</t>
+  </si>
+  <si>
+    <t>TEST-0005</t>
+  </si>
+  <si>
+    <t>TEST-0012</t>
+  </si>
+  <si>
+    <t>TEST-0013</t>
+  </si>
+  <si>
+    <t>GR-0003</t>
+  </si>
+  <si>
+    <t>CLIENT_NAME</t>
+  </si>
+  <si>
+    <t>CLIENT_PREFIX</t>
+  </si>
+  <si>
+    <t>DEVICE_COUNT</t>
+  </si>
+  <si>
+    <t>Good Rest SRL</t>
+  </si>
+  <si>
+    <t>GR</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>0181dd9ee612fddf3ad26f9cbfd412a0</t>
+  </si>
+  <si>
+    <t>FB39AE4BDE08E7329540EBFE4CC3414E</t>
+  </si>
+  <si>
+    <t>754A7D1064611BEAFF3EDF09E6132E25</t>
+  </si>
+  <si>
+    <t>3E74B631BFF9E1A524190ECE8EAB51E7</t>
+  </si>
+  <si>
+    <t>1470EA97AC7204097AD9A4BD83A8F399</t>
+  </si>
+  <si>
+    <t>4318608D344502BE5ECE9241B18B5856</t>
+  </si>
+  <si>
+    <t>663234A0FC88290A62BD4A050E8B5963</t>
+  </si>
+  <si>
+    <t>7D2DDBBADDF9B0DF590182EFE357C387</t>
+  </si>
+  <si>
+    <t>938080278D0289374FDD4C7B2586365C</t>
+  </si>
+  <si>
+    <t>276A0A8BD1D918DA9BD3C39AB6BB6CF1</t>
+  </si>
+  <si>
+    <t>4FF77F2046770BBBC669C28891496EC3</t>
+  </si>
+  <si>
+    <t>BOARD</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -55,7 +265,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -66,6 +280,37 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{371DA425-F10D-414C-933C-3F3A48044E36}" name="DEVICES_TABLE" displayName="DEVICES_TABLE" ref="A1:H16" totalsRowShown="0">
+  <autoFilter ref="A1:H16" xr:uid="{371DA425-F10D-414C-933C-3F3A48044E36}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{DDFDFD3A-0F67-44BC-90CE-8508D1EEF5DF}" name="SERIAL_NUMBER"/>
+    <tableColumn id="2" xr3:uid="{1850FEB3-A6F0-4B5C-BEFD-AEBFC49FCE8C}" name="DEV_EUI"/>
+    <tableColumn id="3" xr3:uid="{0057FAC1-38FD-4174-BDAC-990A1D0E0166}" name="APP_KEY"/>
+    <tableColumn id="4" xr3:uid="{2D3931F4-9DCE-48B8-A238-D47001B95353}" name="VOLTAGE_MEASURED"/>
+    <tableColumn id="5" xr3:uid="{628222F4-9B18-4D85-B022-C2154C1E4FBC}" name="VOLTAGE_REPORTED"/>
+    <tableColumn id="6" xr3:uid="{5CDA7C05-C7A5-4492-8DCA-DC6AE6F51276}" name="CLIENT"/>
+    <tableColumn id="7" xr3:uid="{AEB411F1-B16D-4DC0-90B6-14974ED41593}" name="CLIENT_ID"/>
+    <tableColumn id="8" xr3:uid="{2E42CDED-B7E4-49CD-B60B-AE62A1FC96EA}" name="BOARD"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7395ACB7-E62D-4072-832D-8AA92A2760B2}" name="CLIENTS_TABLE" displayName="CLIENTS_TABLE" ref="A1:C3" totalsRowShown="0">
+  <autoFilter ref="A1:C3" xr:uid="{7395ACB7-E62D-4072-832D-8AA92A2760B2}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{E3B822E9-C8C9-4D12-BA19-6F29D8064867}" name="CLIENT_NAME"/>
+    <tableColumn id="2" xr3:uid="{29B70FAB-7D6D-4297-9136-47776A852A93}" name="CLIENT_PREFIX"/>
+    <tableColumn id="3" xr3:uid="{2BAC8EE9-B5E7-4DDD-84B4-C1CE5E5F426F}" name="DEVICE_COUNT" dataDxfId="0">
+      <calculatedColumnFormula>COUNTIF(DEVICES_TABLE[CLIENT],"="&amp;CLIENTS_TABLE[[#This Row],[CLIENT_NAME]])</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -330,13 +575,445 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E2">
+        <v>3.8180000000000001</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3">
+        <v>3.98</v>
+      </c>
+      <c r="E3">
+        <v>3.6989999999999998</v>
+      </c>
+      <c r="F3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="E4">
+        <v>3.61</v>
+      </c>
+      <c r="F4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5">
+        <v>4.18</v>
+      </c>
+      <c r="E5">
+        <v>3.86</v>
+      </c>
+      <c r="F5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6">
+        <v>4.18</v>
+      </c>
+      <c r="E6">
+        <v>3.86</v>
+      </c>
+      <c r="F6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7">
+        <v>4.18</v>
+      </c>
+      <c r="E7">
+        <v>3.78</v>
+      </c>
+      <c r="F7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" t="s">
+        <v>52</v>
+      </c>
+      <c r="K7" t="str" cm="1">
+        <f t="array" aca="1" ref="K7:K8" ca="1">INDIRECT("CLIENTS_TABLE[CLIENT_NAME]")</f>
+        <v>Good Rest SRL</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" t="str">
+        <f ca="1"/>
+        <v>TEST</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10">
+        <v>4.17</v>
+      </c>
+      <c r="E10">
+        <v>3.72</v>
+      </c>
+      <c r="F10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11">
+        <v>4.17</v>
+      </c>
+      <c r="E11">
+        <v>3.83</v>
+      </c>
+      <c r="F11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12">
+        <v>4.17</v>
+      </c>
+      <c r="E12">
+        <v>3.85</v>
+      </c>
+      <c r="F12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13">
+        <v>4.17</v>
+      </c>
+      <c r="E13">
+        <v>3.87</v>
+      </c>
+      <c r="F13" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" t="s">
+        <v>31</v>
+      </c>
+      <c r="H13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14">
+        <v>4.17</v>
+      </c>
+      <c r="E14">
+        <v>3.82</v>
+      </c>
+      <c r="F14" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F16" xr:uid="{A2CB1A3C-BAF6-4008-8029-88D6EF68FAEB}">
+      <formula1>INDIRECT("CLIENTS_TABLE[CLIENT_NAME]")</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2CE9B66-EAF1-49A7-9C70-602F38D49B8C}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2">
+        <f>COUNTIF(DEVICES_TABLE[CLIENT],"="&amp;CLIENTS_TABLE[[#This Row],[CLIENT_NAME]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3">
+        <f>COUNTIF(DEVICES_TABLE[CLIENT],"="&amp;CLIENTS_TABLE[[#This Row],[CLIENT_NAME]])</f>
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>